<commit_message>
👌 IMPROVE: Summary Features
</commit_message>
<xml_diff>
--- a/workdir/Template_ACI _STE_ADDAX.xlsx
+++ b/workdir/Template_ACI _STE_ADDAX.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugues.nwameh\Desktop\CBC\FILES_ACIs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\herve.ngando\Desktop\labs\eneo\eneo-icn-cashing\workdir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E071F8DA-ABF0-4FDB-8378-0AF5330B1170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A6D4E33-7F2E-4F83-B034-8A263C5CFB55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ACI STE ADDAX" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
     <t>PK_BILL_GENERATED_ID</t>
   </si>
   <si>
-    <t xml:space="preserve">DUE_AMT </t>
+    <t>DUE_AMT</t>
   </si>
 </sst>
 </file>
@@ -997,9 +997,6 @@
     <xf numFmtId="1" fontId="23" fillId="0" borderId="11" xfId="292" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="32" borderId="2" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="20" fillId="0" borderId="0" xfId="30" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1008,6 +1005,9 @@
     <xf numFmtId="3" fontId="20" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="4" fillId="32" borderId="2" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="404">
     <cellStyle name="20 % - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1752,18 +1752,18 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="29.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" style="13" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="29.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1773,203 +1773,203 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="18" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <v>72487214</v>
       </c>
       <c r="B2" s="8">
         <v>203999044</v>
       </c>
-      <c r="C2" s="14">
+      <c r="C2" s="13">
         <v>782622546</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="14">
         <v>116169</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>72487214</v>
       </c>
       <c r="B3" s="9">
         <v>203998951</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="13">
         <v>782621547</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="14">
         <v>60755</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>72487214</v>
       </c>
       <c r="B4" s="8">
         <v>203999001</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="13">
         <v>782615547</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="14">
         <v>100585</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>72487214</v>
       </c>
       <c r="B5" s="8">
         <v>203998865</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="13">
         <v>782609547</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="14">
         <v>69387</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>72487214</v>
       </c>
       <c r="B6" s="8">
         <v>204008962</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="13">
         <v>782617547</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="14">
         <v>70620</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>72487214</v>
       </c>
       <c r="B7" s="8">
         <v>204008941</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="13">
         <v>782622547</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="14">
         <v>81493</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>72487214</v>
       </c>
       <c r="B8" s="10">
         <v>204008990</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="13">
         <v>782613550</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="14">
         <v>2950</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>72487214</v>
       </c>
       <c r="B9" s="10">
         <v>204009009</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="13">
         <v>782608548</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="14">
         <v>64343</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>72487214</v>
       </c>
       <c r="B10" s="11">
         <v>201890613</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="13">
         <v>781463780</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="14">
         <v>540433</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>72487214</v>
       </c>
       <c r="B11" s="11">
         <v>201989476</v>
       </c>
-      <c r="C11" s="17">
+      <c r="C11" s="16">
         <v>781463836</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="17">
         <v>8768508</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7">
         <v>72487214</v>
       </c>
       <c r="B12" s="8">
         <v>203999015</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12" s="13">
         <v>782617964</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="14">
         <v>74207</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7">
         <v>72487214</v>
       </c>
       <c r="B13" s="9">
         <v>204015730</v>
       </c>
-      <c r="C13" s="14">
+      <c r="C13" s="13">
         <v>782611549</v>
       </c>
-      <c r="D13" s="16">
+      <c r="D13" s="15">
         <v>274838</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
         <v>72487214</v>
       </c>
       <c r="B14" s="8">
         <v>203998891</v>
       </c>
-      <c r="C14" s="14">
+      <c r="C14" s="13">
         <v>782624544</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D14" s="15">
         <v>87658</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
         <v>72487214</v>
       </c>
       <c r="B15" s="8">
         <v>203998813</v>
       </c>
-      <c r="C15" s="14">
+      <c r="C15" s="13">
         <v>782619547</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="14">
         <v>58289</v>
       </c>
     </row>

</xml_diff>